<commit_message>
Enhance visitor tracking functionality and add Excel file retrieval
- Updated the VisitTracker component to include 'viewedAtLocal' timestamp.
- Modified the API to append visitor data with the new field and added a GET endpoint to retrieve the visitors.xlsx file.
- Refactored visitorExcel functions for better clarity and added error handling for file retrieval.
</commit_message>
<xml_diff>
--- a/data/visitors.xlsx
+++ b/data/visitors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>timestampIso</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>en-US</t>
+  </si>
+  <si>
+    <t>2026-01-21T07:34:37.311Z</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/144.0.0.0 Safari/537.36</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
@@ -478,8 +484,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>